<commit_message>
Update weekly triaged issues
</commit_message>
<xml_diff>
--- a/spreadsheets/component_stats.xlsx
+++ b/spreadsheets/component_stats.xlsx
@@ -474,14 +474,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ComboBox</t>
+          <t>Popover</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>6</v>
@@ -490,14 +490,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Popover</t>
+          <t>ComboBox</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
         <v>6</v>
@@ -506,14 +506,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tree</t>
+          <t>Dropdown</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>5</v>
@@ -538,14 +538,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dropdown</t>
+          <t>Tree</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>5</v>
@@ -554,39 +554,39 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TagPicker</t>
+          <t>Drawer</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dialog</t>
+          <t>TagPicker</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Drawer</t>
+          <t>Nav</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Toolbar</t>
+          <t>Skeleton</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Nav</t>
+          <t>Tooltip</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Skeleton</t>
+          <t>Toolbar</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,14 +650,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Tooltip</t>
+          <t>Dialog</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
         <v>3</v>
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Portal</t>
+          <t>Virtualizer</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Virtualizer</t>
+          <t>Table</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Table</t>
+          <t>Portal</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,17 +714,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Slider</t>
+          <t>Popup</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SplitButton</t>
+          <t>Avatar</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Popup</t>
+          <t>FocusTrapZone</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,14 +778,14 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Input</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -794,14 +794,14 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Checkbox</t>
+          <t>Button</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>FocusTrapZone</t>
+          <t>InfoLabel</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -858,14 +858,14 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Toast</t>
+          <t>Slider</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SpinButton</t>
+          <t>Switch</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Button</t>
+          <t>Input</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Badge</t>
+          <t>Checkbox</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Switch</t>
+          <t>Badge</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>InfoLabel</t>
+          <t>Toast</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>SpinButton</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Avatar</t>
+          <t>SplitButton</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Coachmark</t>
+          <t>Calendar</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Pickers</t>
+          <t>Keytip</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Carousel</t>
+          <t>Pickers</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Keytip</t>
+          <t>List</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Calendar</t>
+          <t>Coachmark</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>List</t>
+          <t>Carousel</t>
         </is>
       </c>
       <c r="B41" t="n">

</xml_diff>